<commit_message>
Updated dv locker sheet w missing lockers
</commit_message>
<xml_diff>
--- a/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/DVHSLockerCombos.xlsx
+++ b/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/DVHSLockerCombos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishakh/Documents/code/San_Ramon_Makerspace/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D6F329-00E4-054C-A615-258D42EF24B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1AEB2-781F-C748-8F8F-4C91E723DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1240" windowWidth="24840" windowHeight="12220" xr2:uid="{4465FC60-F391-2E4A-ACC7-5675908B3C61}"/>
+    <workbookView xWindow="2580" yWindow="460" windowWidth="24840" windowHeight="12220" xr2:uid="{4465FC60-F391-2E4A-ACC7-5675908B3C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6986" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7034" uniqueCount="346">
   <si>
     <t>31-33-2</t>
   </si>
@@ -1436,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282C0E7B-FDC2-2B43-8B25-680C2D6FB50C}">
-  <dimension ref="A1:E2328"/>
+  <dimension ref="A1:E2344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D359" sqref="D359"/>
+    <sheetView tabSelected="1" topLeftCell="A2326" workbookViewId="0">
+      <selection activeCell="F2343" sqref="F2343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41024,6 +41024,278 @@
         <v>340</v>
       </c>
     </row>
+    <row r="2329" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2329">
+        <v>4146</v>
+      </c>
+      <c r="B2329" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2329">
+        <v>4000</v>
+      </c>
+      <c r="D2329" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2329" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2330">
+        <v>4174</v>
+      </c>
+      <c r="B2330" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2330">
+        <v>4000</v>
+      </c>
+      <c r="D2330" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2330" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2331">
+        <v>4198</v>
+      </c>
+      <c r="B2331" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2331">
+        <v>4000</v>
+      </c>
+      <c r="D2331" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2331" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2332">
+        <v>4025</v>
+      </c>
+      <c r="B2332" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2332">
+        <v>4000</v>
+      </c>
+      <c r="D2332" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2332" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2333">
+        <v>4029</v>
+      </c>
+      <c r="B2333" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2333">
+        <v>4000</v>
+      </c>
+      <c r="D2333" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2333" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2334">
+        <v>4169</v>
+      </c>
+      <c r="B2334" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2334">
+        <v>4000</v>
+      </c>
+      <c r="D2334" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2334" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2335">
+        <v>4171</v>
+      </c>
+      <c r="B2335" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2335">
+        <v>4000</v>
+      </c>
+      <c r="D2335" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2335" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2336">
+        <v>4219</v>
+      </c>
+      <c r="B2336" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2336">
+        <v>4000</v>
+      </c>
+      <c r="D2336" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2336" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2337">
+        <v>4229</v>
+      </c>
+      <c r="B2337" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2337">
+        <v>4000</v>
+      </c>
+      <c r="D2337" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2337" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2338">
+        <v>4247</v>
+      </c>
+      <c r="B2338" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2338">
+        <v>4000</v>
+      </c>
+      <c r="D2338" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2338" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2339">
+        <v>4265</v>
+      </c>
+      <c r="B2339" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2339">
+        <v>4000</v>
+      </c>
+      <c r="D2339" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2339" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2340">
+        <v>4285</v>
+      </c>
+      <c r="B2340" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2340">
+        <v>4000</v>
+      </c>
+      <c r="D2340" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2340" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2341">
+        <v>4291</v>
+      </c>
+      <c r="B2341" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2341">
+        <v>4000</v>
+      </c>
+      <c r="D2341" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2341" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2342">
+        <v>4305</v>
+      </c>
+      <c r="B2342" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2342">
+        <v>4000</v>
+      </c>
+      <c r="D2342" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2342" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2343">
+        <v>4309</v>
+      </c>
+      <c r="B2343" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2343">
+        <v>4000</v>
+      </c>
+      <c r="D2343" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2343" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2344">
+        <v>4317</v>
+      </c>
+      <c r="B2344" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2344">
+        <v>4000</v>
+      </c>
+      <c r="D2344" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2344" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed floors of 4k lockers at the bottom of dv locker sheet
</commit_message>
<xml_diff>
--- a/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/DVHSLockerCombos.xlsx
+++ b/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/DVHSLockerCombos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishakh/Documents/code/San_Ramon_Makerspace/SRVUSD-Lockers/lockers_app/aiohttp_lockers/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1AEB2-781F-C748-8F8F-4C91E723DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6146259D-FB1E-8944-B5A3-EDB7D35FAD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="460" windowWidth="24840" windowHeight="12220" xr2:uid="{4465FC60-F391-2E4A-ACC7-5675908B3C61}"/>
   </bookViews>
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:E2344"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2326" workbookViewId="0">
-      <selection activeCell="F2343" sqref="F2343"/>
+      <selection activeCell="E2338" sqref="E2338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41035,7 +41035,7 @@
         <v>4000</v>
       </c>
       <c r="D2329" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2329" t="s">
         <v>341</v>
@@ -41052,7 +41052,7 @@
         <v>4000</v>
       </c>
       <c r="D2330" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2330" t="s">
         <v>341</v>
@@ -41069,7 +41069,7 @@
         <v>4000</v>
       </c>
       <c r="D2331" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2331" t="s">
         <v>341</v>
@@ -41086,7 +41086,7 @@
         <v>4000</v>
       </c>
       <c r="D2332" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2332" t="s">
         <v>341</v>
@@ -41103,7 +41103,7 @@
         <v>4000</v>
       </c>
       <c r="D2333" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2333" t="s">
         <v>341</v>
@@ -41120,7 +41120,7 @@
         <v>4000</v>
       </c>
       <c r="D2334" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2334" t="s">
         <v>341</v>
@@ -41137,7 +41137,7 @@
         <v>4000</v>
       </c>
       <c r="D2335" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2335" t="s">
         <v>341</v>
@@ -41154,7 +41154,7 @@
         <v>4000</v>
       </c>
       <c r="D2336" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2336" t="s">
         <v>341</v>
@@ -41171,7 +41171,7 @@
         <v>4000</v>
       </c>
       <c r="D2337" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2337" t="s">
         <v>341</v>
@@ -41188,7 +41188,7 @@
         <v>4000</v>
       </c>
       <c r="D2338" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2338" t="s">
         <v>341</v>
@@ -41205,7 +41205,7 @@
         <v>4000</v>
       </c>
       <c r="D2339" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2339" t="s">
         <v>341</v>
@@ -41222,7 +41222,7 @@
         <v>4000</v>
       </c>
       <c r="D2340" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2340" t="s">
         <v>341</v>
@@ -41239,7 +41239,7 @@
         <v>4000</v>
       </c>
       <c r="D2341" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2341" t="s">
         <v>341</v>
@@ -41256,7 +41256,7 @@
         <v>4000</v>
       </c>
       <c r="D2342" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2342" t="s">
         <v>341</v>
@@ -41273,7 +41273,7 @@
         <v>4000</v>
       </c>
       <c r="D2343" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2343" t="s">
         <v>341</v>
@@ -41290,7 +41290,7 @@
         <v>4000</v>
       </c>
       <c r="D2344" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E2344" t="s">
         <v>341</v>

</xml_diff>